<commit_message>
minor changes runorder xl file
</commit_message>
<xml_diff>
--- a/Resource_TestData/RunOrder.xlsx
+++ b/Resource_TestData/RunOrder.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="16005" windowHeight="5820"/>
+    <workbookView xWindow="5670" yWindow="3855" windowWidth="17790" windowHeight="5025"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>TestCase_ID</t>
   </si>
@@ -40,13 +40,25 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Testcase001</t>
-  </si>
-  <si>
-    <t>Testcase002</t>
-  </si>
-  <si>
-    <t>Testcase003</t>
+    <t>login_with_correct_credentials</t>
+  </si>
+  <si>
+    <t>login_with_invalid_credentials</t>
+  </si>
+  <si>
+    <t>login_and_place_an_order</t>
+  </si>
+  <si>
+    <t>login_as_manager_and_check_manager_able_to_login_or_not</t>
+  </si>
+  <si>
+    <t>login_as_counter_and_place_an_order</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>test5</t>
   </si>
 </sst>
 </file>
@@ -390,17 +402,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="57.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -445,6 +457,28 @@
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>